<commit_message>
arreglo al archivo de casos de pruebas
</commit_message>
<xml_diff>
--- a/casos_de_prueba.xlsx
+++ b/casos_de_prueba.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -105,10 +105,7 @@
     <t>editar perfil 2 veces</t>
   </si>
   <si>
-    <t xml:space="preserve">genera un error en el template de page not found </t>
-  </si>
-  <si>
-    <t>no</t>
+    <t>genera un error en el template de page not found - pequeño delay en la carga de la web 3 segundos deslogea y todo ok</t>
   </si>
 </sst>
 </file>
@@ -526,7 +523,7 @@
   <dimension ref="A2:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +670,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
casos de prueba de fran
</commit_message>
<xml_diff>
--- a/casos_de_prueba.xlsx
+++ b/casos_de_prueba.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive\Escritorio\probando cosas del proyecto\entregaFinal\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EB02EB-C20C-4DF7-B5EC-E83463EBC5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28515" windowHeight="12855"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -106,12 +112,33 @@
   </si>
   <si>
     <t>genera un error en el template de page not found - pequeño delay en la carga de la web 3 segundos deslogea y todo ok</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>consultas</t>
+  </si>
+  <si>
+    <t>el formulario de consulta funciona correctamente</t>
+  </si>
+  <si>
+    <t>visualizacion de consultas</t>
+  </si>
+  <si>
+    <t>las consultas solo se ven en el perfil de un superuser donde aparecen los datos que envio la persona en el formulario</t>
+  </si>
+  <si>
+    <t>Allen/Rio Negro</t>
+  </si>
+  <si>
+    <t>los comentarios de cargan correctamente y se visualizan solo en el curso donde se realizo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -219,24 +246,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{0457EAE5-EDAE-487D-B8D4-EAFA2A155927}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -274,7 +307,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -346,7 +379,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -519,11 +552,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +862,9 @@
       <c r="C26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
@@ -855,31 +890,61 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="11">
+        <v>45217</v>
+      </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="A30" s="1">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="11">
+        <v>45218</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="A31" s="1">
+        <v>3</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="11">
+        <v>45219</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -888,7 +953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -900,7 +965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>